<commit_message>
Adding project details documentation to git
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>S.No.</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>Verify the search results when search with 'data catalog' text by selecting other categories.</t>
+  </si>
+  <si>
+    <t>Verify that Paperback/Hardcover/kindle book types are getting displayed in Product details page</t>
+  </si>
+  <si>
+    <t>Verify that new book price and old book price (if available) are getting displayed in Paperback tab.</t>
+  </si>
+  <si>
+    <t>Verify that Kindle book details (Price, book features etc) are getting displayed after clicking on 'Kindle' tab in Product details page.</t>
+  </si>
+  <si>
+    <t>Verify that selected book details (Book title, authors, Book available types etc) are getting displayed in Product details page.</t>
+  </si>
+  <si>
+    <t>Verify that Paperback/Hardcover is displayed by default after navgating to Product details page.</t>
   </si>
 </sst>
 </file>
@@ -397,16 +412,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="93" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="119.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -454,13 +467,41 @@
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>